<commit_message>
SCTE&VT marks validation for MP cases
</commit_message>
<xml_diff>
--- a/target/test-classes/dataSheets/Book2.xlsx
+++ b/target/test-classes/dataSheets/Book2.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$1521</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -5136,11 +5139,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1521"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1521"/>
+    <sheetView tabSelected="1" topLeftCell="A280" workbookViewId="0">
+      <selection activeCell="A299" sqref="A299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -21874,6 +21880,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C1521"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>